<commit_message>
Uploaded Updated Utility file
Added Updated Utility file with corrected Object Repository
</commit_message>
<xml_diff>
--- a/SampleScript/Utility/SeleniumUtility.xlsx
+++ b/SampleScript/Utility/SeleniumUtility.xlsx
@@ -198,9 +198,6 @@
     <t>E:\Open2Test\Open2Test_Selenium\SampleScript\TestCase\</t>
   </si>
   <si>
-    <t>E:\Open2Test\Open2Test_Selenium\SampleScript\TestOR\TestObjectItemsList.xlsx</t>
-  </si>
-  <si>
     <t>E:\Open2Test\Open2Test_Selenium\SampleScript\report\</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>E:\Open2Test\Open2Test_Selenium\SampleScript\Driver\</t>
+  </si>
+  <si>
+    <t>E:\Open2Test\Open2Test_Selenium\SampleScript\TestOR\DemoOR.xlsx</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -788,7 +788,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -850,7 +850,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -882,7 +882,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -946,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>

</xml_diff>